<commit_message>
tables of the winding configurations
</commit_message>
<xml_diff>
--- a/Project_2/winding.xlsx
+++ b/Project_2/winding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\EE568\Project_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB607BAE-1D40-405E-A24A-658F93C4D873}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B34C2C7-7DCC-43FE-9AE4-776E93DA9523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24825" activeTab="1" xr2:uid="{4E9FF1D6-D4E8-4B3A-B3EC-48B09DE5BACE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="66">
   <si>
     <t>q</t>
   </si>
@@ -160,18 +160,141 @@
     <t>4/6 pitched</t>
   </si>
   <si>
-    <t>düz</t>
-  </si>
-  <si>
-    <t>ters</t>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>w</t>
+    </r>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fifth</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>third</t>
+  </si>
+  <si>
+    <t>fifth</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>reverse</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Phase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,16 +338,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,12 +667,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBF7D50-3FDA-4CB4-AB89-249D1921DDF1}">
   <dimension ref="A2:Y58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -603,7 +734,7 @@
       <c r="T3" t="s">
         <v>6</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="4">
         <f>SIN(R5*R6/2)/R5/SIN(R6/2)</f>
         <v>0.83652549231433648</v>
       </c>
@@ -668,7 +799,7 @@
       <c r="T4" t="s">
         <v>7</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="4">
         <f>SIN(3*R5*R6/2)/R5/SIN(R6*3/2)</f>
         <v>3.2758749587986036E-5</v>
       </c>
@@ -697,7 +828,7 @@
       <c r="T5" t="s">
         <v>8</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="4">
         <f>SIN(R5*R6*5/2)/R5/SIN(R6*5/2)</f>
         <v>-0.22416616815249923</v>
       </c>
@@ -758,7 +889,7 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>0.96592782463641236</v>
       </c>
       <c r="H10" t="s">
@@ -770,7 +901,7 @@
       <c r="J10" t="s">
         <v>12</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="4">
         <v>0.96592782359988882</v>
       </c>
     </row>
@@ -784,7 +915,7 @@
       <c r="F11" t="s">
         <v>7</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>0.7071231599922605</v>
       </c>
       <c r="H11" t="s">
@@ -796,7 +927,7 @@
       <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>-0.7071231531630251</v>
       </c>
     </row>
@@ -810,7 +941,7 @@
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <v>0.25885633511600659</v>
       </c>
       <c r="H12" t="s">
@@ -822,7 +953,7 @@
       <c r="J12" t="s">
         <v>14</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="4">
         <v>0.25885632817162912</v>
       </c>
     </row>
@@ -842,7 +973,18 @@
         <v>3.1415000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>49</v>
+      </c>
+      <c r="S16" t="s">
+        <v>47</v>
+      </c>
+      <c r="T16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -879,8 +1021,20 @@
       <c r="L17">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>44</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0.96592782463641236</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0.7071231599922605</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0.25885633511600659</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -917,8 +1071,20 @@
       <c r="L18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>45</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0.86600996110644468</v>
+      </c>
+      <c r="S18" s="4">
+        <v>9.2653589660046209E-5</v>
+      </c>
+      <c r="T18" s="4">
+        <v>-0.86610260478318479</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -955,18 +1121,30 @@
       <c r="L19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>46</v>
+      </c>
+      <c r="R19" s="5">
+        <v>0.83650311784501219</v>
+      </c>
+      <c r="S19" s="4">
+        <v>6.5517499105038104E-5</v>
+      </c>
+      <c r="T19" s="4">
+        <v>-0.22419614610860228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>3</v>
       </c>
@@ -974,7 +1152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1178,7 @@
         <v>0.96592782359988882</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>5</v>
       </c>
@@ -1026,7 +1204,7 @@
         <v>-0.7071231531630251</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1230,7 @@
         <v>0.25885632817162912</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>1</v>
       </c>
@@ -1060,7 +1238,7 @@
         <v>0.52358333333333329</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>2</v>
       </c>
@@ -1068,7 +1246,7 @@
         <v>3.1415000000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1106,7 +1284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1522,36 +1700,46 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6699F6F-883D-4FDE-AF41-2CAE09600D84}">
-  <dimension ref="A2:Y8"/>
+  <dimension ref="A2:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1559,8 +1747,15 @@
         <f>360/C2*C3/2</f>
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>360/D2*D3/2</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
@@ -1597,46 +1792,10 @@
       <c r="M6">
         <v>12</v>
       </c>
-      <c r="N6">
-        <v>13</v>
-      </c>
-      <c r="O6">
-        <v>14</v>
-      </c>
-      <c r="P6">
-        <v>15</v>
-      </c>
-      <c r="Q6">
-        <v>16</v>
-      </c>
-      <c r="R6">
-        <v>17</v>
-      </c>
-      <c r="S6">
-        <v>18</v>
-      </c>
-      <c r="T6">
-        <v>19</v>
-      </c>
-      <c r="U6">
-        <v>20</v>
-      </c>
-      <c r="V6">
-        <v>21</v>
-      </c>
-      <c r="W6">
-        <v>22</v>
-      </c>
-      <c r="X6">
-        <v>23</v>
-      </c>
-      <c r="Y6">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -1685,58 +1844,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="N7" s="1">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="O7" s="1">
-        <f t="shared" si="0"/>
-        <v>345</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="0"/>
-        <v>315</v>
-      </c>
-      <c r="R7" s="2">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="S7" s="2">
-        <f t="shared" si="0"/>
-        <v>285</v>
-      </c>
-      <c r="T7" s="2">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="U7" s="2">
-        <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="V7" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="W7" s="3">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="X7" s="3">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="Y7" s="3">
-        <f t="shared" si="0"/>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1">
         <f>MOD(B7+180,360)</f>
@@ -1786,53 +1897,1164 @@
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="N8" s="1">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
         <v>0</v>
       </c>
-      <c r="O8" s="1">
-        <f t="shared" si="1"/>
+      <c r="C9">
+        <f>MOD(B9+165*3,360)</f>
+        <v>135</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:M9" si="2">MOD(C9+165*3,360)</f>
+        <v>270</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>315</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>MOD(B10+165*5,360)</f>
+        <v>105</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:M10" si="3">MOD(C10+165*5,360)</f>
+        <v>210</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>315</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
         <v>165</v>
       </c>
-      <c r="P8" s="1">
-        <f t="shared" si="1"/>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>270</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
         <v>330</v>
       </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="1"/>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>18</v>
+      </c>
+      <c r="H13">
+        <v>19</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>21</v>
+      </c>
+      <c r="K13">
+        <v>22</v>
+      </c>
+      <c r="L13">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1">
+        <f>MOD(M7+165,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C14" s="1">
+        <f>MOD(B14+165,360)</f>
+        <v>345</v>
+      </c>
+      <c r="D14" s="1">
+        <f>MOD(C14+165,360)</f>
+        <v>150</v>
+      </c>
+      <c r="E14" s="1">
+        <f>MOD(D14+165,360)</f>
+        <v>315</v>
+      </c>
+      <c r="F14" s="2">
+        <f>MOD(E14+165,360)</f>
+        <v>120</v>
+      </c>
+      <c r="G14" s="2">
+        <f>MOD(F14+165,360)</f>
+        <v>285</v>
+      </c>
+      <c r="H14" s="2">
+        <f>MOD(G14+165,360)</f>
+        <v>90</v>
+      </c>
+      <c r="I14" s="2">
+        <f>MOD(H14+165,360)</f>
+        <v>255</v>
+      </c>
+      <c r="J14" s="3">
+        <f>MOD(I14+165,360)</f>
+        <v>60</v>
+      </c>
+      <c r="K14" s="3">
+        <f>MOD(J14+165,360)</f>
+        <v>225</v>
+      </c>
+      <c r="L14" s="3">
+        <f>MOD(K14+165,360)</f>
+        <v>30</v>
+      </c>
+      <c r="M14" s="3">
+        <f>MOD(L14+165,360)</f>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1">
+        <f>MOD(B14+180,360)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <f>MOD(C14+180,360)</f>
+        <v>165</v>
+      </c>
+      <c r="D15" s="1">
+        <f>MOD(D14+180,360)</f>
+        <v>330</v>
+      </c>
+      <c r="E15" s="1">
+        <f>MOD(E14+180,360)</f>
         <v>135</v>
       </c>
-      <c r="R8" s="2">
-        <f t="shared" si="1"/>
+      <c r="F15" s="2">
+        <f>MOD(F14+180,360)</f>
         <v>300</v>
       </c>
-      <c r="S8" s="2">
-        <f t="shared" si="1"/>
+      <c r="G15" s="2">
+        <f>MOD(G14+180,360)</f>
         <v>105</v>
       </c>
-      <c r="T8" s="2">
-        <f t="shared" si="1"/>
+      <c r="H15" s="2">
+        <f>MOD(H14+180,360)</f>
         <v>270</v>
       </c>
-      <c r="U8" s="2">
-        <f t="shared" si="1"/>
+      <c r="I15" s="2">
+        <f>MOD(I14+180,360)</f>
         <v>75</v>
       </c>
-      <c r="V8" s="3">
-        <f t="shared" si="1"/>
+      <c r="J15" s="3">
+        <f>MOD(J14+180,360)</f>
         <v>240</v>
       </c>
-      <c r="W8" s="3">
-        <f t="shared" si="1"/>
+      <c r="K15" s="3">
+        <f>MOD(K14+180,360)</f>
         <v>45</v>
       </c>
-      <c r="X8" s="3">
-        <f t="shared" si="1"/>
+      <c r="L15" s="3">
+        <f>MOD(L14+180,360)</f>
         <v>210</v>
       </c>
-      <c r="Y8" s="3">
-        <f t="shared" si="1"/>
+      <c r="M15" s="3">
+        <f>MOD(M14+180,360)</f>
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <f>MOD(M9+165*3,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C16">
+        <f>MOD(B16+165*3,360)</f>
+        <v>315</v>
+      </c>
+      <c r="D16">
+        <f>MOD(C16+165*3,360)</f>
+        <v>90</v>
+      </c>
+      <c r="E16">
+        <f>MOD(D16+165*3,360)</f>
+        <v>225</v>
+      </c>
+      <c r="F16">
+        <f>MOD(E16+165*3,360)</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>MOD(F16+165*3,360)</f>
+        <v>135</v>
+      </c>
+      <c r="H16">
+        <f>MOD(G16+165*3,360)</f>
+        <v>270</v>
+      </c>
+      <c r="I16">
+        <f>MOD(H16+165*3,360)</f>
+        <v>45</v>
+      </c>
+      <c r="J16">
+        <f>MOD(I16+165*3,360)</f>
+        <v>180</v>
+      </c>
+      <c r="K16">
+        <f>MOD(J16+165*3,360)</f>
+        <v>315</v>
+      </c>
+      <c r="L16">
+        <f>MOD(K16+165*3,360)</f>
+        <v>90</v>
+      </c>
+      <c r="M16">
+        <f>MOD(L16+165*3,360)</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <f>MOD(M10+165*5,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C17">
+        <f>MOD(B17+165*5,360)</f>
+        <v>285</v>
+      </c>
+      <c r="D17">
+        <f>MOD(C17+165*5,360)</f>
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <f>MOD(D17+165*5,360)</f>
+        <v>135</v>
+      </c>
+      <c r="F17">
+        <f>MOD(E17+165*5,360)</f>
+        <v>240</v>
+      </c>
+      <c r="G17">
+        <f>MOD(F17+165*5,360)</f>
+        <v>345</v>
+      </c>
+      <c r="H17">
+        <f>MOD(G17+165*5,360)</f>
+        <v>90</v>
+      </c>
+      <c r="I17">
+        <f>MOD(H17+165*5,360)</f>
+        <v>195</v>
+      </c>
+      <c r="J17">
+        <f>MOD(I17+165*5,360)</f>
+        <v>300</v>
+      </c>
+      <c r="K17">
+        <f>MOD(J17+165*5,360)</f>
+        <v>45</v>
+      </c>
+      <c r="L17">
+        <f>MOD(K17+165*5,360)</f>
+        <v>150</v>
+      </c>
+      <c r="M17">
+        <f>MOD(L17+165*5,360)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22">
+        <v>9</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22">
+        <v>11</v>
+      </c>
+      <c r="M22">
+        <v>12</v>
+      </c>
+      <c r="N22">
+        <v>13</v>
+      </c>
+      <c r="O22">
+        <v>14</v>
+      </c>
+      <c r="P22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <f>MOD(B23+132,360)</f>
+        <v>132</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" ref="D23:AE23" si="4">MOD(C23+132,360)</f>
+        <v>264</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="4"/>
+        <v>168</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="4"/>
+        <v>204</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="4"/>
+        <v>336</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="4"/>
+        <v>276</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1">
+        <f>MOD(B23+180,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:AE24" si="5">MOD(C23+180,360)</f>
+        <v>312</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="5"/>
+        <v>216</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="5"/>
+        <v>348</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="5"/>
+        <v>252</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="5"/>
+        <v>156</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="5"/>
+        <v>288</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="5"/>
+        <v>324</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="5"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>MOD(B25+132*3,360)</f>
+        <v>36</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:P25" si="6">MOD(C25+132*3,360)</f>
+        <v>72</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="6"/>
+        <v>144</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>216</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>252</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>288</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>324</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="6"/>
+        <v>72</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="6"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>MOD(B26+132*5,360)</f>
+        <v>300</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:P26" si="7">MOD(C26+132*5,360)</f>
+        <v>240</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J27" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" t="s">
+        <v>60</v>
+      </c>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>57</v>
+      </c>
+      <c r="O27" t="s">
+        <v>58</v>
+      </c>
+      <c r="P27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>17</v>
+      </c>
+      <c r="D29">
+        <v>18</v>
+      </c>
+      <c r="E29">
+        <v>19</v>
+      </c>
+      <c r="F29">
+        <v>20</v>
+      </c>
+      <c r="G29">
+        <v>21</v>
+      </c>
+      <c r="H29">
+        <v>22</v>
+      </c>
+      <c r="I29">
+        <v>23</v>
+      </c>
+      <c r="J29">
+        <v>24</v>
+      </c>
+      <c r="K29">
+        <v>25</v>
+      </c>
+      <c r="L29">
+        <v>26</v>
+      </c>
+      <c r="M29">
+        <v>27</v>
+      </c>
+      <c r="N29">
+        <v>28</v>
+      </c>
+      <c r="O29">
+        <v>29</v>
+      </c>
+      <c r="P29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="1">
+        <f>MOD(P23+132,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C30" s="1">
+        <f>MOD(B30+132,360)</f>
+        <v>312</v>
+      </c>
+      <c r="D30" s="2">
+        <f>MOD(C30+132,360)</f>
+        <v>84</v>
+      </c>
+      <c r="E30" s="3">
+        <f>MOD(D30+132,360)</f>
+        <v>216</v>
+      </c>
+      <c r="F30" s="1">
+        <f>MOD(E30+132,360)</f>
+        <v>348</v>
+      </c>
+      <c r="G30" s="2">
+        <f>MOD(F30+132,360)</f>
+        <v>120</v>
+      </c>
+      <c r="H30" s="2">
+        <f>MOD(G30+132,360)</f>
+        <v>252</v>
+      </c>
+      <c r="I30" s="3">
+        <f>MOD(H30+132,360)</f>
+        <v>24</v>
+      </c>
+      <c r="J30" s="1">
+        <f>MOD(I30+132,360)</f>
+        <v>156</v>
+      </c>
+      <c r="K30" s="2">
+        <f>MOD(J30+132,360)</f>
+        <v>288</v>
+      </c>
+      <c r="L30" s="3">
+        <f>MOD(K30+132,360)</f>
+        <v>60</v>
+      </c>
+      <c r="M30" s="3">
+        <f>MOD(L30+132,360)</f>
+        <v>192</v>
+      </c>
+      <c r="N30" s="1">
+        <f>MOD(M30+132,360)</f>
+        <v>324</v>
+      </c>
+      <c r="O30" s="2">
+        <f>MOD(N30+132,360)</f>
+        <v>96</v>
+      </c>
+      <c r="P30" s="3">
+        <f>MOD(O30+132,360)</f>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1">
+        <f>MOD(B30+180,360)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <f>MOD(C30+180,360)</f>
+        <v>132</v>
+      </c>
+      <c r="D31" s="2">
+        <f>MOD(D30+180,360)</f>
+        <v>264</v>
+      </c>
+      <c r="E31" s="3">
+        <f>MOD(E30+180,360)</f>
+        <v>36</v>
+      </c>
+      <c r="F31" s="1">
+        <f>MOD(F30+180,360)</f>
+        <v>168</v>
+      </c>
+      <c r="G31" s="2">
+        <f>MOD(G30+180,360)</f>
+        <v>300</v>
+      </c>
+      <c r="H31" s="2">
+        <f>MOD(H30+180,360)</f>
+        <v>72</v>
+      </c>
+      <c r="I31" s="3">
+        <f>MOD(I30+180,360)</f>
+        <v>204</v>
+      </c>
+      <c r="J31" s="1">
+        <f>MOD(J30+180,360)</f>
+        <v>336</v>
+      </c>
+      <c r="K31" s="2">
+        <f>MOD(K30+180,360)</f>
+        <v>108</v>
+      </c>
+      <c r="L31" s="3">
+        <f>MOD(L30+180,360)</f>
+        <v>240</v>
+      </c>
+      <c r="M31" s="3">
+        <f>MOD(M30+180,360)</f>
+        <v>12</v>
+      </c>
+      <c r="N31" s="1">
+        <f>MOD(N30+180,360)</f>
+        <v>144</v>
+      </c>
+      <c r="O31" s="2">
+        <f>MOD(O30+180,360)</f>
+        <v>276</v>
+      </c>
+      <c r="P31" s="3">
+        <f>MOD(P30+180,360)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <f>MOD(P25+132*3,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C32">
+        <f>MOD(B32+132*3,360)</f>
+        <v>216</v>
+      </c>
+      <c r="D32">
+        <f>MOD(C32+132*3,360)</f>
+        <v>252</v>
+      </c>
+      <c r="E32">
+        <f>MOD(D32+132*3,360)</f>
+        <v>288</v>
+      </c>
+      <c r="F32">
+        <f>MOD(E32+132*3,360)</f>
+        <v>324</v>
+      </c>
+      <c r="G32">
+        <f>MOD(F32+132*3,360)</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>MOD(G32+132*3,360)</f>
+        <v>36</v>
+      </c>
+      <c r="I32">
+        <f>MOD(H32+132*3,360)</f>
+        <v>72</v>
+      </c>
+      <c r="J32">
+        <f>MOD(I32+132*3,360)</f>
+        <v>108</v>
+      </c>
+      <c r="K32">
+        <f>MOD(J32+132*3,360)</f>
+        <v>144</v>
+      </c>
+      <c r="L32">
+        <f>MOD(K32+132*3,360)</f>
+        <v>180</v>
+      </c>
+      <c r="M32">
+        <f>MOD(L32+132*3,360)</f>
+        <v>216</v>
+      </c>
+      <c r="N32">
+        <f>MOD(M32+132*3,360)</f>
+        <v>252</v>
+      </c>
+      <c r="O32">
+        <f>MOD(N32+132*3,360)</f>
+        <v>288</v>
+      </c>
+      <c r="P32">
+        <f>MOD(O32+132*3,360)</f>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <f>MOD(P26+132*5,360)</f>
+        <v>180</v>
+      </c>
+      <c r="C33">
+        <f>MOD(B33+132*5,360)</f>
+        <v>120</v>
+      </c>
+      <c r="D33">
+        <f>MOD(C33+132*5,360)</f>
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <f>MOD(D33+132*5,360)</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f>MOD(E33+132*5,360)</f>
+        <v>300</v>
+      </c>
+      <c r="G33">
+        <f>MOD(F33+132*5,360)</f>
+        <v>240</v>
+      </c>
+      <c r="H33">
+        <f>MOD(G33+132*5,360)</f>
+        <v>180</v>
+      </c>
+      <c r="I33">
+        <f>MOD(H33+132*5,360)</f>
+        <v>120</v>
+      </c>
+      <c r="J33">
+        <f>MOD(I33+132*5,360)</f>
+        <v>60</v>
+      </c>
+      <c r="K33">
+        <f>MOD(J33+132*5,360)</f>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <f>MOD(K33+132*5,360)</f>
+        <v>300</v>
+      </c>
+      <c r="M33">
+        <f>MOD(L33+132*5,360)</f>
+        <v>240</v>
+      </c>
+      <c r="N33">
+        <f>MOD(M33+132*5,360)</f>
+        <v>180</v>
+      </c>
+      <c r="O33">
+        <f>MOD(N33+132*5,360)</f>
+        <v>120</v>
+      </c>
+      <c r="P33">
+        <f>MOD(O33+132*5,360)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" t="s">
+        <v>58</v>
+      </c>
+      <c r="I34" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" t="s">
+        <v>57</v>
+      </c>
+      <c r="K34" t="s">
+        <v>58</v>
+      </c>
+      <c r="L34" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" t="s">
+        <v>60</v>
+      </c>
+      <c r="N34" t="s">
+        <v>56</v>
+      </c>
+      <c r="O34" t="s">
+        <v>59</v>
+      </c>
+      <c r="P34" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>